<commit_message>
rédaction rapport d'analyse en cours
</commit_message>
<xml_diff>
--- a/documentation/Checklist+Audit+SEO+2018.xlsx
+++ b/documentation/Checklist+Audit+SEO+2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\outils_code\local_repo\VictorDauphin_4_27042021\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C6D813-CB1F-4739-A99A-F235161F6952}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F1440E-91A1-491D-93C1-937598052D3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="checklist préalable" sheetId="1" r:id="rId1"/>
@@ -477,6 +477,65 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -490,65 +549,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1161,7 +1161,7 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55:D56"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1173,246 +1173,246 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="16" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="20"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="12" t="s">
         <v>52</v>
       </c>
       <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="18"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="12" t="s">
         <v>55</v>
       </c>
       <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20" t="s">
+      <c r="C17" s="8"/>
+      <c r="D17" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="27" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15" t="s">
+      <c r="C19" s="12"/>
+      <c r="D19" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="20"/>
+      <c r="D21" s="14"/>
     </row>
     <row r="22" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="15"/>
     </row>
     <row r="23" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="16" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="18"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="15"/>
     </row>
     <row r="25" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20" t="s">
+      <c r="C25" s="8"/>
+      <c r="D25" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="15"/>
     </row>
     <row r="27" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="12" t="s">
         <v>65</v>
       </c>
       <c r="D27" s="16" t="s">
@@ -1420,40 +1420,40 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="15"/>
     </row>
     <row r="29" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="26" t="s">
+      <c r="D29" s="14"/>
+      <c r="E29" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="13"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="26" t="s">
+      <c r="A30" s="11"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="4" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="12" t="s">
         <v>70</v>
       </c>
       <c r="C31" s="16" t="s">
@@ -1462,207 +1462,207 @@
       <c r="D31" s="16"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
     </row>
     <row r="33" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="20"/>
+      <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="18"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="15"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="12" t="s">
         <v>73</v>
       </c>
       <c r="D35" s="16"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="13"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="18"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="15"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="14" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="13"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="18"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="15"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="12" t="s">
         <v>75</v>
       </c>
       <c r="D39" s="16"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="13"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="18"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="15"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="14" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="18"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="15"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="15"/>
+      <c r="C43" s="12"/>
       <c r="D43" s="16" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="13"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="18"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="15"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D45" s="20" t="s">
+      <c r="D45" s="14" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="13"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="18"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="15"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B47" s="28" t="s">
+      <c r="B47" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="29" t="s">
+      <c r="C47" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D47" s="30" t="s">
+      <c r="D47" s="23" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="25"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="23"/>
+      <c r="A48" s="18"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="22"/>
       <c r="D48" s="24"/>
     </row>
     <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C49" s="15"/>
+      <c r="C49" s="12"/>
       <c r="D49" s="16"/>
     </row>
     <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="13"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="18"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="15"/>
     </row>
     <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D51" s="20" t="s">
+      <c r="D51" s="14" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="13"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="18"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="15"/>
     </row>
     <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="12" t="s">
         <v>91</v>
       </c>
       <c r="D53" s="16" t="s">
@@ -1670,79 +1670,61 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="13"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="18"/>
+      <c r="A54" s="11"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="15"/>
     </row>
     <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="10"/>
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="20"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="14"/>
     </row>
     <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="13"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="18"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="112">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="C37:C38"/>
@@ -1765,42 +1747,60 @@
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:D18 A21:D28 A19:B20 D19:D20">
     <cfRule type="expression" dxfId="6" priority="4">
@@ -1852,295 +1852,295 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="14"/>
     </row>
     <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="14"/>
     </row>
     <row r="18" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="15"/>
     </row>
     <row r="19" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="20"/>
+      <c r="D21" s="14"/>
     </row>
     <row r="22" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="15"/>
     </row>
     <row r="23" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="16"/>
     </row>
     <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="18"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="15"/>
     </row>
     <row r="25" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="14"/>
     </row>
     <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="15"/>
     </row>
     <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="16"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="15"/>
     </row>
     <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="14"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="15"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="16"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="18"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="15"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="14" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="18"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="15"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B35" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="12" t="s">
         <v>98</v>
       </c>
       <c r="D35" s="16" t="s">
@@ -2148,105 +2148,169 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="13"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="31"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="18"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="15"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="14" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="13"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="18"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="15"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="15"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="16"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="13"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="18"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="15"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="6"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="27"/>
     </row>
     <row r="42" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="7"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="28"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="30"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="13"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="7"/>
+      <c r="A44" s="11"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="28"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="6"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="27"/>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="13"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="7"/>
+      <c r="A46" s="11"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="28"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="14"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="9"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="30"/>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="13"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="7"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="96">
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
     <mergeCell ref="C43:C44"/>
@@ -2263,81 +2327,17 @@
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:D48">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2364,211 +2364,259 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="14" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="15"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="14"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="16"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="15"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="14"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="16"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="15"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="15"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="14"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="18"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="15"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="16"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="15"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="20"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="14"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="15"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="16"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="13"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="60">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="C29:C30"/>
@@ -2581,62 +2629,14 @@
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:D8">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:D30">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>